<commit_message>
WASH app edits to test system
</commit_message>
<xml_diff>
--- a/WASH_shiny.xlsx
+++ b/WASH_shiny.xlsx
@@ -5,26 +5,28 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lclem\OneDrive\Documents\GitHub\plhR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/018fd3f915004678/Documents/GitHub/plhR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E55AD6C-B94C-4B0E-8EC5-8C02F1845C10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{C13C494B-8FE0-42BA-8EE0-EF199D111E54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="731" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="731" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="contents" sheetId="2" r:id="rId1"/>
     <sheet name="demographics" sheetId="1" r:id="rId2"/>
     <sheet name="td_engagement" sheetId="10" r:id="rId3"/>
     <sheet name="td_eng_completed" sheetId="9" r:id="rId4"/>
-    <sheet name="td_eng_started" sheetId="11" r:id="rId5"/>
+    <sheet name="td_eng_completed_toggle" sheetId="13" r:id="rId5"/>
+    <sheet name="td_eng_started" sheetId="11" r:id="rId6"/>
+    <sheet name="td_eng_started_toggle" sheetId="12" r:id="rId7"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="119">
   <si>
     <t>type</t>
   </si>
@@ -119,42 +121,6 @@
     <t>boxplot_table</t>
   </si>
   <si>
-    <t>rp.contact.field.safe_food_completed</t>
-  </si>
-  <si>
-    <t>rp.contact.field.handwashing_with_soap_completed</t>
-  </si>
-  <si>
-    <t>rp.contact.field.introduction_completed</t>
-  </si>
-  <si>
-    <t>rp.contact.field.safe_drinking_water_completed</t>
-  </si>
-  <si>
-    <t>rp.contact.field.waste_completed</t>
-  </si>
-  <si>
-    <t>rp.contact.field.celebration_completed</t>
-  </si>
-  <si>
-    <t>rp.contact.field.bathing_completed</t>
-  </si>
-  <si>
-    <t>rp.contact.field.healthy_families_completed</t>
-  </si>
-  <si>
-    <t>rp.contact.field.when_to_wash_your_hands_completed</t>
-  </si>
-  <si>
-    <t>rp.contact.field.clean_toilets_completed</t>
-  </si>
-  <si>
-    <t>rp.contact.field.healthy_homes_completed</t>
-  </si>
-  <si>
-    <t>rp.contact.field.how_to_wash_your_hands_completed</t>
-  </si>
-  <si>
     <t>box5</t>
   </si>
   <si>
@@ -227,10 +193,196 @@
     <t>td_eng_completed</t>
   </si>
   <si>
-    <t>introduction_started</t>
-  </si>
-  <si>
-    <t>text = "Started Introduction", colour = "orange"</t>
+    <t>text = "Started Introduction", colour = "blue"</t>
+  </si>
+  <si>
+    <t>text = "Started Safe Food", colour = "blue"</t>
+  </si>
+  <si>
+    <t>text = "Started Handwashing", colour = "blue"</t>
+  </si>
+  <si>
+    <t>text = "Started Safe Drinking Water", colour = "blue"</t>
+  </si>
+  <si>
+    <t>text = "Started Waste", colour = "blue"</t>
+  </si>
+  <si>
+    <t>text = "Started Celebration", colour = "blue"</t>
+  </si>
+  <si>
+    <t>text = "Started Bathing", colour = "blue"</t>
+  </si>
+  <si>
+    <t>text = "Started Healthy Families", colour = "blue"</t>
+  </si>
+  <si>
+    <t>text = "Started When to Wash Hands", colour = "blue"</t>
+  </si>
+  <si>
+    <t>text = "Started Clean Toilets", colour = "blue"</t>
+  </si>
+  <si>
+    <t>text = "Started Healthy Homes", colour = "blue"</t>
+  </si>
+  <si>
+    <t>text = "Started How to Wash Hands", colour = "blue"</t>
+  </si>
+  <si>
+    <t>Started (Toggle)</t>
+  </si>
+  <si>
+    <t>td_eng_started_toggle</t>
+  </si>
+  <si>
+    <t>introduction_started_not_toggle</t>
+  </si>
+  <si>
+    <t>safe_food_started_not_toggle</t>
+  </si>
+  <si>
+    <t>handwashing_with_soap_started_not_toggle</t>
+  </si>
+  <si>
+    <t>safe_drinking_water_started_not_toggle</t>
+  </si>
+  <si>
+    <t>waste_started_not_toggle</t>
+  </si>
+  <si>
+    <t>celebration_started_not_toggle</t>
+  </si>
+  <si>
+    <t>bathing_started_not_toggle</t>
+  </si>
+  <si>
+    <t>healthy_families_started_not_toggle</t>
+  </si>
+  <si>
+    <t>when_to_wash_your_hands_started_not_toggle</t>
+  </si>
+  <si>
+    <t>clean_toilets_started_not_toggle</t>
+  </si>
+  <si>
+    <t>healthy_homes_started_not_toggle</t>
+  </si>
+  <si>
+    <t>how_to_wash_your_hands_started_not_toggle</t>
+  </si>
+  <si>
+    <t>introduction_started_toggle</t>
+  </si>
+  <si>
+    <t>safe_food_started_toggle</t>
+  </si>
+  <si>
+    <t>handwashing_with_soap_started_toggle</t>
+  </si>
+  <si>
+    <t>safe_drinking_water_started_toggle</t>
+  </si>
+  <si>
+    <t>waste_started_toggle</t>
+  </si>
+  <si>
+    <t>celebration_started_toggle</t>
+  </si>
+  <si>
+    <t>bathing_started_toggle</t>
+  </si>
+  <si>
+    <t>healthy_families_started_toggle</t>
+  </si>
+  <si>
+    <t>when_to_wash_your_hands_started_toggle</t>
+  </si>
+  <si>
+    <t>clean_toilets_started_toggle</t>
+  </si>
+  <si>
+    <t>healthy_homes_started_toggle</t>
+  </si>
+  <si>
+    <t>how_to_wash_your_hands_started_toggle</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>td_eng_completed_toggle</t>
+  </si>
+  <si>
+    <t>introduction_completed_toggle</t>
+  </si>
+  <si>
+    <t>safe_food_completed_toggle</t>
+  </si>
+  <si>
+    <t>handwashing_with_soap_completed_toggle</t>
+  </si>
+  <si>
+    <t>safe_drinking_water_completed_toggle</t>
+  </si>
+  <si>
+    <t>waste_completed_toggle</t>
+  </si>
+  <si>
+    <t>celebration_completed_toggle</t>
+  </si>
+  <si>
+    <t>bathing_completed_toggle</t>
+  </si>
+  <si>
+    <t>healthy_families_completed_toggle</t>
+  </si>
+  <si>
+    <t>when_to_wash_your_hands_completed_toggle</t>
+  </si>
+  <si>
+    <t>clean_toilets_completed_toggle</t>
+  </si>
+  <si>
+    <t>healthy_homes_completed_toggle</t>
+  </si>
+  <si>
+    <t>how_to_wash_your_hands_completed_toggle</t>
+  </si>
+  <si>
+    <t>introduction_completed_not_toggle</t>
+  </si>
+  <si>
+    <t>safe_food_completed_not_toggle</t>
+  </si>
+  <si>
+    <t>handwashing_with_soap_completed_not_toggle</t>
+  </si>
+  <si>
+    <t>safe_drinking_water_completed_not_toggle</t>
+  </si>
+  <si>
+    <t>waste_completed_not_toggle</t>
+  </si>
+  <si>
+    <t>celebration_completed_not_toggle</t>
+  </si>
+  <si>
+    <t>bathing_completed_not_toggle</t>
+  </si>
+  <si>
+    <t>healthy_families_completed_not_toggle</t>
+  </si>
+  <si>
+    <t>when_to_wash_your_hands_completed_not_toggle</t>
+  </si>
+  <si>
+    <t>clean_toilets_completed_not_toggle</t>
+  </si>
+  <si>
+    <t>healthy_homes_completed_not_toggle</t>
+  </si>
+  <si>
+    <t>how_to_wash_your_hands_completed_not_toggle</t>
   </si>
 </sst>
 </file>
@@ -815,10 +967,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF152DC1-4175-4A08-98B6-9875CE538BB3}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -839,24 +991,46 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
         <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>66</v>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -868,8 +1042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C63DAF98-772F-4DFA-8572-31F09E1E6A1F}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="A1:G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -910,10 +1084,10 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>33</v>
+        <v>107</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -927,10 +1101,10 @@
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>31</v>
+        <v>108</v>
       </c>
       <c r="G3">
         <v>4</v>
@@ -944,10 +1118,10 @@
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>32</v>
+        <v>109</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -961,10 +1135,10 @@
         <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>34</v>
+        <v>110</v>
       </c>
       <c r="G5">
         <v>3</v>
@@ -975,13 +1149,13 @@
         <v>19</v>
       </c>
       <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" t="s">
         <v>43</v>
       </c>
-      <c r="D6" t="s">
-        <v>55</v>
-      </c>
       <c r="E6" s="2" t="s">
-        <v>35</v>
+        <v>111</v>
       </c>
       <c r="G6">
         <v>4</v>
@@ -992,13 +1166,13 @@
         <v>19</v>
       </c>
       <c r="B7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" t="s">
         <v>44</v>
       </c>
-      <c r="D7" t="s">
-        <v>56</v>
-      </c>
       <c r="E7" s="2" t="s">
-        <v>36</v>
+        <v>112</v>
       </c>
       <c r="G7">
         <v>6</v>
@@ -1009,13 +1183,13 @@
         <v>19</v>
       </c>
       <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" t="s">
         <v>45</v>
       </c>
-      <c r="D8" t="s">
-        <v>57</v>
-      </c>
       <c r="E8" s="2" t="s">
-        <v>37</v>
+        <v>113</v>
       </c>
       <c r="G8">
         <v>6</v>
@@ -1026,13 +1200,13 @@
         <v>19</v>
       </c>
       <c r="B9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" t="s">
         <v>46</v>
       </c>
-      <c r="D9" t="s">
-        <v>58</v>
-      </c>
       <c r="E9" s="2" t="s">
-        <v>38</v>
+        <v>114</v>
       </c>
       <c r="G9">
         <v>3</v>
@@ -1043,13 +1217,13 @@
         <v>19</v>
       </c>
       <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" t="s">
         <v>47</v>
       </c>
-      <c r="D10" t="s">
-        <v>59</v>
-      </c>
       <c r="E10" s="2" t="s">
-        <v>39</v>
+        <v>115</v>
       </c>
       <c r="G10">
         <v>2</v>
@@ -1060,13 +1234,13 @@
         <v>19</v>
       </c>
       <c r="B11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" t="s">
         <v>48</v>
       </c>
-      <c r="D11" t="s">
-        <v>60</v>
-      </c>
       <c r="E11" s="2" t="s">
-        <v>40</v>
+        <v>116</v>
       </c>
       <c r="G11">
         <v>5</v>
@@ -1077,13 +1251,13 @@
         <v>19</v>
       </c>
       <c r="B12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" t="s">
         <v>49</v>
       </c>
-      <c r="D12" t="s">
-        <v>61</v>
-      </c>
       <c r="E12" s="2" t="s">
-        <v>41</v>
+        <v>117</v>
       </c>
       <c r="G12">
         <v>5</v>
@@ -1094,13 +1268,13 @@
         <v>19</v>
       </c>
       <c r="B13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" t="s">
         <v>50</v>
       </c>
-      <c r="D13" t="s">
-        <v>62</v>
-      </c>
       <c r="E13" s="3" t="s">
-        <v>42</v>
+        <v>118</v>
       </c>
       <c r="G13">
         <v>2</v>
@@ -1113,11 +1287,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCF14D57-0BE2-4D81-A4A6-F122E72BED91}">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA1CC97C-CAD1-465E-AE96-2C034F6B7FC0}">
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1153,13 +1327,685 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>67</v>
+        <v>95</v>
       </c>
       <c r="G2">
         <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="G6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="G9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="G11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="G13">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCF14D57-0BE2-4D81-A4A6-F122E72BED91}">
+  <dimension ref="A1:G13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" t="s">
+        <v>65</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" t="s">
+        <v>66</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G13">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A80786C0-93AB-482A-9BF1-EF3E9BEE8E3A}">
+  <dimension ref="A1:G13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="G10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="G11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" t="s">
+        <v>65</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" t="s">
+        <v>66</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="G13">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding ability to read listed table
</commit_message>
<xml_diff>
--- a/WASH_shiny.xlsx
+++ b/WASH_shiny.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/018fd3f915004678/Documents/GitHub/plhR/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lclem\OneDrive\Documents\GitHub\plhR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{C13C494B-8FE0-42BA-8EE0-EF199D111E54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED859BA7-D324-4169-9155-76810127CE19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="731" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="731" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="contents" sheetId="2" r:id="rId1"/>
@@ -20,13 +20,15 @@
     <sheet name="td_eng_completed_toggle" sheetId="13" r:id="rId5"/>
     <sheet name="td_eng_started" sheetId="11" r:id="rId6"/>
     <sheet name="td_eng_started_toggle" sheetId="12" r:id="rId7"/>
+    <sheet name="td_modules" sheetId="14" r:id="rId8"/>
+    <sheet name="td_modules_started" sheetId="15" r:id="rId9"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="124">
   <si>
     <t>type</t>
   </si>
@@ -383,13 +385,28 @@
   </si>
   <si>
     <t>how_to_wash_your_hands_completed_not_toggle</t>
+  </si>
+  <si>
+    <t>Modules</t>
+  </si>
+  <si>
+    <t>td_modules</t>
+  </si>
+  <si>
+    <t>td_modules_started</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>mod_compl_nt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -418,6 +435,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF000000"/>
+      <name val="Lucida Console"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -445,7 +468,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -454,6 +477,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -794,7 +820,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{870FAA04-D1DA-469D-A43D-8817AEA92C36}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
@@ -847,6 +873,20 @@
         <v>22</v>
       </c>
       <c r="D3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4" t="s">
         <v>21</v>
       </c>
     </row>
@@ -970,7 +1010,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1042,7 +1082,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C63DAF98-772F-4DFA-8572-31F09E1E6A1F}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -1533,7 +1573,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection sqref="A1:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2011,4 +2051,125 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2137D2B-4CCD-4240-B497-71AEC5867C95}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AF59F33-DB76-4BC9-93A0-DA4FB6A22DCC}">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="38.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
code updates - adding download tab functionality
</commit_message>
<xml_diff>
--- a/WASH_shiny.xlsx
+++ b/WASH_shiny.xlsx
@@ -1,34 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/018fd3f915004678/Documents/GitHub/plhR/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lclem\OneDrive\Documents\GitHub\plhR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{ED859BA7-D324-4169-9155-76810127CE19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{56A31885-7362-4998-B074-A54CE5919DF2}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A961433-F44A-48D0-B768-3972D002C6CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="731" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="731" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="contents" sheetId="2" r:id="rId1"/>
-    <sheet name="demographics" sheetId="1" r:id="rId2"/>
-    <sheet name="td_engagement" sheetId="10" r:id="rId3"/>
-    <sheet name="td_eng_completed" sheetId="9" r:id="rId4"/>
-    <sheet name="td_eng_completed_toggle" sheetId="13" r:id="rId5"/>
-    <sheet name="td_eng_started" sheetId="11" r:id="rId6"/>
-    <sheet name="td_eng_started_toggle" sheetId="12" r:id="rId7"/>
-    <sheet name="td_modules" sheetId="14" r:id="rId8"/>
-    <sheet name="td_modules_started" sheetId="15" r:id="rId9"/>
+    <sheet name="download2" sheetId="17" r:id="rId2"/>
+    <sheet name="download" sheetId="16" r:id="rId3"/>
+    <sheet name="demographics" sheetId="1" r:id="rId4"/>
+    <sheet name="td_engagement" sheetId="10" r:id="rId5"/>
+    <sheet name="td_eng_completed" sheetId="9" r:id="rId6"/>
+    <sheet name="td_eng_completed_toggle" sheetId="13" r:id="rId7"/>
+    <sheet name="td_eng_started" sheetId="11" r:id="rId8"/>
+    <sheet name="td_eng_started_toggle" sheetId="12" r:id="rId9"/>
+    <sheet name="td_modules" sheetId="14" r:id="rId10"/>
+    <sheet name="td_modules_started" sheetId="15" r:id="rId11"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="145">
   <si>
     <t>type</t>
   </si>
@@ -399,9 +401,6 @@
     <t>data</t>
   </si>
   <si>
-    <t>mod_compl_nt</t>
-  </si>
-  <si>
     <t>bar_freq</t>
   </si>
   <si>
@@ -409,6 +408,63 @@
   </si>
   <si>
     <t>boxplot_summary</t>
+  </si>
+  <si>
+    <t>text = "One on one time", colour = "blue"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">one_on_one_teen </t>
+  </si>
+  <si>
+    <t>flow_checkin_data</t>
+  </si>
+  <si>
+    <t>text = "Praise", colour = "blue"</t>
+  </si>
+  <si>
+    <t>praise_teen</t>
+  </si>
+  <si>
+    <t>filter_variable</t>
+  </si>
+  <si>
+    <t>filter_value</t>
+  </si>
+  <si>
+    <t>response</t>
+  </si>
+  <si>
+    <t>Download</t>
+  </si>
+  <si>
+    <t>download</t>
+  </si>
+  <si>
+    <t>Data label</t>
+  </si>
+  <si>
+    <t>Download label</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>df</t>
+  </si>
+  <si>
+    <t>Format</t>
+  </si>
+  <si>
+    <t>Data to download:</t>
+  </si>
+  <si>
+    <t>csv</t>
+  </si>
+  <si>
+    <t>iris</t>
+  </si>
+  <si>
+    <t>mtcars</t>
   </si>
 </sst>
 </file>
@@ -795,11 +851,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{870FAA04-D1DA-469D-A43D-8817AEA92C36}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -865,17 +919,301 @@
         <v>21</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>134</v>
+      </c>
+      <c r="B5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C5" t="s">
+        <v>135</v>
+      </c>
+      <c r="D5" t="s">
+        <v>135</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2137D2B-4CCD-4240-B497-71AEC5867C95}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AF59F33-DB76-4BC9-93A0-DA4FB6A22DCC}">
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="38.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>129</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" t="s">
+        <v>130</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{032D77F8-1038-4979-A255-54443A8E5533}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B5" t="s">
+        <v>144</v>
+      </c>
+      <c r="C5" t="s">
+        <v>144</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E7B9A43-AE69-497D-83D5-13D43404AED7}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.90625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>138</v>
+      </c>
+      <c r="B6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C6" t="s">
+        <v>143</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C1" sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -883,6 +1221,7 @@
     <col min="1" max="1" width="18" customWidth="1"/>
     <col min="3" max="3" width="9.1796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43.90625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -928,7 +1267,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
@@ -945,7 +1284,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
@@ -962,7 +1301,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
@@ -999,7 +1338,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF152DC1-4175-4A08-98B6-9875CE538BB3}">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -1072,7 +1411,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C63DAF98-772F-4DFA-8572-31F09E1E6A1F}">
   <dimension ref="A1:G13"/>
   <sheetViews>
@@ -1320,7 +1659,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA1CC97C-CAD1-465E-AE96-2C034F6B7FC0}">
   <dimension ref="A1:G13"/>
   <sheetViews>
@@ -1562,7 +1901,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCF14D57-0BE2-4D81-A4A6-F122E72BED91}">
   <dimension ref="A1:G13"/>
   <sheetViews>
@@ -1805,7 +2144,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A80786C0-93AB-482A-9BF1-EF3E9BEE8E3A}">
   <dimension ref="A1:G13"/>
   <sheetViews>
@@ -2045,125 +2384,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2137D2B-4CCD-4240-B497-71AEC5867C95}">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AF59F33-DB76-4BC9-93A0-DA4FB6A22DCC}">
-  <dimension ref="A1:H3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="4" max="4" width="38.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.1796875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3" t="s">
-        <v>123</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
implementation of filter checkboxes in shiny dshboard
</commit_message>
<xml_diff>
--- a/WASH_shiny.xlsx
+++ b/WASH_shiny.xlsx
@@ -5,32 +5,31 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lclem\OneDrive\Documents\GitHub\plhR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/018fd3f915004678/Documents/GitHub/plhR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A961433-F44A-48D0-B768-3972D002C6CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{3DADF427-5147-4EF1-A667-884414FE2E92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="731" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="731" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="contents" sheetId="2" r:id="rId1"/>
-    <sheet name="download2" sheetId="17" r:id="rId2"/>
-    <sheet name="download" sheetId="16" r:id="rId3"/>
-    <sheet name="demographics" sheetId="1" r:id="rId4"/>
-    <sheet name="td_engagement" sheetId="10" r:id="rId5"/>
-    <sheet name="td_eng_completed" sheetId="9" r:id="rId6"/>
-    <sheet name="td_eng_completed_toggle" sheetId="13" r:id="rId7"/>
-    <sheet name="td_eng_started" sheetId="11" r:id="rId8"/>
-    <sheet name="td_eng_started_toggle" sheetId="12" r:id="rId9"/>
-    <sheet name="td_modules" sheetId="14" r:id="rId10"/>
-    <sheet name="td_modules_started" sheetId="15" r:id="rId11"/>
+    <sheet name="main_page" sheetId="16" r:id="rId2"/>
+    <sheet name="demographics" sheetId="1" r:id="rId3"/>
+    <sheet name="td_engagement" sheetId="10" r:id="rId4"/>
+    <sheet name="td_eng_completed" sheetId="9" r:id="rId5"/>
+    <sheet name="td_eng_completed_toggle" sheetId="13" r:id="rId6"/>
+    <sheet name="td_eng_started" sheetId="11" r:id="rId7"/>
+    <sheet name="td_eng_started_toggle" sheetId="12" r:id="rId8"/>
+    <sheet name="td_modules" sheetId="14" r:id="rId9"/>
+    <sheet name="td_modules_started" sheetId="15" r:id="rId10"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="164">
   <si>
     <t>type</t>
   </si>
@@ -434,37 +433,94 @@
     <t>response</t>
   </si>
   <si>
-    <t>Download</t>
-  </si>
-  <si>
-    <t>download</t>
-  </si>
-  <si>
-    <t>Data label</t>
-  </si>
-  <si>
-    <t>Download label</t>
-  </si>
-  <si>
-    <t>Data</t>
-  </si>
-  <si>
-    <t>df</t>
-  </si>
-  <si>
-    <t>Format</t>
-  </si>
-  <si>
-    <t>Data to download:</t>
-  </si>
-  <si>
-    <t>csv</t>
-  </si>
-  <si>
-    <t>iris</t>
-  </si>
-  <si>
-    <t>mtcars</t>
+    <t>value_box</t>
+  </si>
+  <si>
+    <t>myvaluebox1</t>
+  </si>
+  <si>
+    <t>text = "Joined", colour = "yellow", icon = "user"</t>
+  </si>
+  <si>
+    <t>joined</t>
+  </si>
+  <si>
+    <t>myvaluebox2</t>
+  </si>
+  <si>
+    <t>text = "Enrolled", colour = "purple", icon = "clipboard"</t>
+  </si>
+  <si>
+    <t>enrolled</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>myvaluebox3</t>
+  </si>
+  <si>
+    <t>text = "Completed Onboarding", colour = "aqua", icon = "check"</t>
+  </si>
+  <si>
+    <t>completed_onboarding</t>
+  </si>
+  <si>
+    <t>myvaluebox4</t>
+  </si>
+  <si>
+    <t>text = "Active in last 24 hours", colour = "green", icon = "clock"</t>
+  </si>
+  <si>
+    <t>active_in_last_24_hours</t>
+  </si>
+  <si>
+    <t>myvaluebox5</t>
+  </si>
+  <si>
+    <t>text = "Active in last 7 days", colour = "orange", icon = "calendar"</t>
+  </si>
+  <si>
+    <t>active_in_last_7_days</t>
+  </si>
+  <si>
+    <t>mean_box</t>
+  </si>
+  <si>
+    <t>myvaluebox6</t>
+  </si>
+  <si>
+    <t>text = "Average days in the chatbot", colour = "orange", icon = "active"</t>
+  </si>
+  <si>
+    <t>time_in_study_n</t>
+  </si>
+  <si>
+    <t>myvaluebox7</t>
+  </si>
+  <si>
+    <t>text = "Average goals completed (%)", colour = "aqua", icon = "bullseye"</t>
+  </si>
+  <si>
+    <t>perc_goals_completed</t>
+  </si>
+  <si>
+    <t>myvaluebox8</t>
+  </si>
+  <si>
+    <t>text = "Average modules completed (%)", colour = "purple", icon = "star"</t>
+  </si>
+  <si>
+    <t>perc_modules_completed</t>
+  </si>
+  <si>
+    <t>checkbox_group</t>
+  </si>
+  <si>
+    <t>checkbox_test</t>
+  </si>
+  <si>
+    <t>label = "User Enrolled", choices = c("Yes" = "yes", "No" = "no")</t>
   </si>
 </sst>
 </file>
@@ -562,6 +618,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -851,9 +911,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{870FAA04-D1DA-469D-A43D-8817AEA92C36}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -919,61 +981,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>134</v>
-      </c>
-      <c r="B5" t="s">
-        <v>134</v>
-      </c>
-      <c r="C5" t="s">
-        <v>135</v>
-      </c>
-      <c r="D5" t="s">
-        <v>135</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2137D2B-4CCD-4240-B497-71AEC5867C95}">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AF59F33-DB76-4BC9-93A0-DA4FB6A22DCC}">
   <dimension ref="A1:I3"/>
   <sheetViews>
@@ -1073,59 +1086,172 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{032D77F8-1038-4979-A255-54443A8E5533}">
-  <dimension ref="A1:C5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{457D521C-A218-4630-A92D-9512A3F85D41}">
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D2" t="s">
         <v>136</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D3" t="s">
+        <v>139</v>
+      </c>
+      <c r="E3" t="s">
+        <v>140</v>
+      </c>
+      <c r="F3" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>137</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
+        <v>142</v>
+      </c>
+      <c r="D4" t="s">
+        <v>143</v>
+      </c>
+      <c r="E4" t="s">
+        <v>144</v>
+      </c>
+      <c r="F4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>134</v>
+      </c>
+      <c r="B5" t="s">
+        <v>145</v>
+      </c>
+      <c r="D5" t="s">
+        <v>146</v>
+      </c>
+      <c r="E5" t="s">
+        <v>147</v>
+      </c>
+      <c r="F5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B6" t="s">
+        <v>148</v>
+      </c>
+      <c r="D6" t="s">
+        <v>149</v>
+      </c>
+      <c r="E6" t="s">
+        <v>150</v>
+      </c>
+      <c r="F6" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>151</v>
+      </c>
+      <c r="B7" t="s">
+        <v>152</v>
+      </c>
+      <c r="D7" t="s">
+        <v>153</v>
+      </c>
+      <c r="E7" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>151</v>
+      </c>
+      <c r="B8" t="s">
+        <v>155</v>
+      </c>
+      <c r="D8" t="s">
+        <v>156</v>
+      </c>
+      <c r="E8" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>151</v>
+      </c>
+      <c r="B9" t="s">
+        <v>158</v>
+      </c>
+      <c r="D9" t="s">
+        <v>159</v>
+      </c>
+      <c r="E9" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>161</v>
+      </c>
+      <c r="B10" t="s">
+        <v>162</v>
+      </c>
+      <c r="D10" t="s">
+        <v>163</v>
+      </c>
+      <c r="E10" t="s">
         <v>140</v>
-      </c>
-      <c r="C4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>138</v>
-      </c>
-      <c r="B5" t="s">
-        <v>144</v>
-      </c>
-      <c r="C5" t="s">
-        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -1134,86 +1260,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E7B9A43-AE69-497D-83D5-13D43404AED7}">
-  <dimension ref="A1:C6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="13.90625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>136</v>
-      </c>
-      <c r="B2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>137</v>
-      </c>
-      <c r="B3" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>140</v>
-      </c>
-      <c r="C4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>138</v>
-      </c>
-      <c r="B5" t="s">
-        <v>139</v>
-      </c>
-      <c r="C5" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>138</v>
-      </c>
-      <c r="B6" t="s">
-        <v>143</v>
-      </c>
-      <c r="C6" t="s">
-        <v>143</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C1" sqref="A1:C1"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1338,7 +1389,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF152DC1-4175-4A08-98B6-9875CE538BB3}">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -1411,7 +1462,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C63DAF98-772F-4DFA-8572-31F09E1E6A1F}">
   <dimension ref="A1:G13"/>
   <sheetViews>
@@ -1659,7 +1710,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA1CC97C-CAD1-465E-AE96-2C034F6B7FC0}">
   <dimension ref="A1:G13"/>
   <sheetViews>
@@ -1901,7 +1952,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCF14D57-0BE2-4D81-A4A6-F122E72BED91}">
   <dimension ref="A1:G13"/>
   <sheetViews>
@@ -2144,7 +2195,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A80786C0-93AB-482A-9BF1-EF3E9BEE8E3A}">
   <dimension ref="A1:G13"/>
   <sheetViews>
@@ -2384,4 +2435,39 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2137D2B-4CCD-4240-B497-71AEC5867C95}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
WASH_shiny1 example xlsx file
</commit_message>
<xml_diff>
--- a/WASH_shiny.xlsx
+++ b/WASH_shiny.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lclem\OneDrive\Documents\GitHub\plhR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/018fd3f915004678/Documents/GitHub/plhR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA2F4FC3-E41F-495C-9674-ADE3BECF9B19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="6_{CACD6F31-85E6-4FCA-844A-0C4DDE616D53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{87525488-B6CF-4E9F-969E-0410EC6AB51F}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="731" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11280" tabRatio="731" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="contents" sheetId="2" r:id="rId1"/>
@@ -1086,10 +1086,18 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="F10" sqref="A1:F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="61.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -1254,6 +1262,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1262,7 +1271,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>